<commit_message>
fix resolution issue for tap item
</commit_message>
<xml_diff>
--- a/DB/db.xlsx
+++ b/DB/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db211ccea624a480/Documents/GitHub/Evn-Automation-tool/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="114_{2B503599-1001-4CE6-9DD1-55E21E6033A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B54D8AC-9CD7-41DB-B9C2-5CF8627E2D15}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="114_{2B503599-1001-4CE6-9DD1-55E21E6033A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAC376F4-9CA0-44F5-AFD1-5098383828EB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="1020" windowWidth="21600" windowHeight="6315" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companion" sheetId="44" r:id="rId1"/>
@@ -3289,7 +3289,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update automation tool structure
</commit_message>
<xml_diff>
--- a/DB/db.xlsx
+++ b/DB/db.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db211ccea624a480/Documents/GitHub/Evn-Automation-tool/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="114_{2B503599-1001-4CE6-9DD1-55E21E6033A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAC376F4-9CA0-44F5-AFD1-5098383828EB}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="114_{2B503599-1001-4CE6-9DD1-55E21E6033A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{362EE11B-8A3B-4A10-BA81-1206A377E82C}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="1020" windowWidth="21600" windowHeight="6315" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companion" sheetId="44" r:id="rId1"/>
-    <sheet name="GoldenApple" sheetId="48" r:id="rId2"/>
-    <sheet name="UI" sheetId="47" r:id="rId3"/>
-    <sheet name="Pet" sheetId="4" r:id="rId4"/>
-    <sheet name="Cheat" sheetId="46" r:id="rId5"/>
-    <sheet name="Mount" sheetId="45" r:id="rId6"/>
+    <sheet name="UI" sheetId="47" r:id="rId2"/>
+    <sheet name="Pet" sheetId="4" r:id="rId3"/>
+    <sheet name="Cheat" sheetId="46" r:id="rId4"/>
+    <sheet name="Mount" sheetId="45" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_1._조건제_보상_추가_패키지">#REF!</definedName>
@@ -61,11 +60,11 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Giang Vu Truong [evan] - Personal View" guid="{92D4AFAD-54DB-4804-87A5-F807BA99876A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="20"/>
+    <customWorkbookView name="Lam Thi Hong Dao [jennie] - Personal View" guid="{B24583BA-3210-4EBE-B061-E5EC220FA01C}" mergeInterval="0" personalView="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="이지수  - 사용자 보기" guid="{C4F271E8-9872-4292-ACEB-11725380EC57}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="73" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Doan Quang Trung [wright] - Personal View" guid="{446B9943-40F4-4499-B266-AC8AE7CCE110}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="6"/>
     <customWorkbookView name="Tran Bao Ngoc [beca] - Personal View" guid="{F1A9B88A-78B1-419F-A391-83B1454A44C5}" mergeInterval="0" personalView="1" xWindow="118" yWindow="404" windowWidth="1802" windowHeight="676" tabRatio="679" activeSheetId="10"/>
-    <customWorkbookView name="Doan Quang Trung [wright] - Personal View" guid="{446B9943-40F4-4499-B266-AC8AE7CCE110}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="6"/>
-    <customWorkbookView name="이지수  - 사용자 보기" guid="{C4F271E8-9872-4292-ACEB-11725380EC57}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="73" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Lam Thi Hong Dao [jennie] - Personal View" guid="{B24583BA-3210-4EBE-B061-E5EC220FA01C}" mergeInterval="0" personalView="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Giang Vu Truong [evan] - Personal View" guid="{92D4AFAD-54DB-4804-87A5-F807BA99876A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="20"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -186,114 +185,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Mohammad Ally [wolverine]</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2A7A2A18-BC99-424A-AFAD-BBC9704A85C6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mohammad Ally [wolverine]:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Link with Configuration file (MUST HAVE and UNIQUE)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{FF6D0550-FBB7-42C4-A006-E1E2178AD808}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mohammad Ally [wolverine]:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Use in Report file only (for human to read)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{71BE212E-C2B8-42FB-BD3B-BA97816508CA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mohammad Ally [wolverine]:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Use in Report file only (for human to read)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{8F73C2CF-6398-49CF-A827-A3FDE6A4A06C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mohammad Ally [wolverine]:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Image Database (folder), IMAGE MUST EXIST in folder.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="251">
   <si>
     <t>Path</t>
   </si>
@@ -947,27 +840,6 @@
   </si>
   <si>
     <t>In-game Navigation UI</t>
-  </si>
-  <si>
-    <t>GoldApple_auto-battle charge ticket (30 min)</t>
-  </si>
-  <si>
-    <t>GoldApple_berzerker bon-bons</t>
-  </si>
-  <si>
-    <t>GoldApple_bottomless hp potion v2.0</t>
-  </si>
-  <si>
-    <t>GoldApple_fruity candy</t>
-  </si>
-  <si>
-    <t>GoldApple_Net's Pyramid Admission Ticket</t>
-  </si>
-  <si>
-    <t>GoldApple_Nett's pyramid Entry ticket</t>
-  </si>
-  <si>
-    <t>Mysterious weapon wheatstone (rare)</t>
   </si>
   <si>
     <t>UI_btn_Buy1</t>
@@ -1073,7 +945,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1121,28 +993,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1155,14 +1007,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1250,41 +1096,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1305,18 +1121,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1950,17 +1754,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D73BA-C301-47A9-B5A2-51E4ECFCF070}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="4" width="30.625" customWidth="1"/>
     <col min="5" max="5" width="87.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>187</v>
       </c>
@@ -1977,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1995,7 +1799,7 @@
         <v>/Companions/Fellow_Evelyn.png</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2013,7 +1817,7 @@
         <v>/Companions/Fellow_Milia.png</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2031,7 +1835,7 @@
         <v>/Companions/Fellow_Cassel.png</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2049,7 +1853,7 @@
         <v>/Companions/Fellow_Latz.png</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2067,7 +1871,7 @@
         <v>/Companions/Fellow_Human_OldMan.png</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2085,7 +1889,7 @@
         <v>/Companions/Fellow_Human_Woman.png</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2103,7 +1907,7 @@
         <v>/Companions/Fellow_Human_Girl.png</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2121,7 +1925,7 @@
         <v>/Companions/Fellow_Human_FatMan.png</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2139,7 +1943,7 @@
         <v>/Companions/Fellow_Human_Man.png</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2157,7 +1961,7 @@
         <v>/Companions/Fellow_Echo_Boy.png</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2175,7 +1979,7 @@
         <v>/Companions/Fellow_Thief.png</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2193,7 +1997,7 @@
         <v>/Companions/Fellow_Echo_Man.png</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2211,7 +2015,7 @@
         <v>/Companions/Fellow_CitizenAristocrat.png</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2229,7 +2033,7 @@
         <v>/Companions/Fellow_Echo_Guard.png</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2247,7 +2051,7 @@
         <v>/Companions/Fellow_HumanBoy.png</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2265,7 +2069,7 @@
         <v>/Companions/Fellow_CitizenWoman.png</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2283,7 +2087,7 @@
         <v>/Companions/Fellow_DrakeOldMan.png</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2301,7 +2105,7 @@
         <v>/Companions/Fellow_DrakeOldWoman.png</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2319,7 +2123,7 @@
         <v>/Companions/Fellow_DrakeGuard.png</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2337,7 +2141,7 @@
         <v>/Companions/Fellow_DrakeGirl.png</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2355,7 +2159,7 @@
         <v>/Companions/Fellow_Human_Guard.png</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2373,7 +2177,7 @@
         <v>/Companions/Fellow_PengKintMerchant.png</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2391,7 +2195,7 @@
         <v>/Companions/Fellow_GrocerShop.png</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2409,7 +2213,7 @@
         <v>/Companions/Fellow_PengKintAlchemist.png</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2427,7 +2231,7 @@
         <v>/Companions/Fellow_Equipment.png</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2445,7 +2249,7 @@
         <v>/Companions/Fellow_Collection.png</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2463,7 +2267,7 @@
         <v>/Companions/Fellow_Orc.png</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2481,7 +2285,7 @@
         <v>/Companions/Fellow_Hunter_Woman.png</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2499,7 +2303,7 @@
         <v>/Companions/Fellow_Echo_Woman.png</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2517,7 +2321,7 @@
         <v>/Companions/Fellow_Echo_Girl.png</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2535,7 +2339,7 @@
         <v>/Companions/Fellow_TraceDismantler.png</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2553,7 +2357,7 @@
         <v>/Companions/Fellow_Human_ManFarmer.png</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2571,7 +2375,7 @@
         <v>/Companions/Fellow_Human_WomanFarmer.png</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2589,7 +2393,7 @@
         <v>/Companions/Fellow_DrakeMan.png</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2607,7 +2411,7 @@
         <v>/Companions/Fellow_DrakeWoman.png</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2625,7 +2429,7 @@
         <v>/Companions/Fellow_Human_ChiefGuard.png</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2643,7 +2447,7 @@
         <v>/Companions/Fellow_DrakeElder.png</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2661,7 +2465,7 @@
         <v>/Companions/Fellow_Human_Boy.png</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2679,7 +2483,7 @@
         <v>/Companions/Fellow_GuildAdministrator.png</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2697,7 +2501,7 @@
         <v>/Companions/Fellow_Drake_Jeweller.png</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2715,7 +2519,7 @@
         <v>/Companions/Fellow_Hunter_Man.png</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2733,7 +2537,7 @@
         <v>/Companions/Fellow_Echo_ChiefGuard.png</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2751,7 +2555,7 @@
         <v>/Companions/Fellow_SkillBookMerchant.png</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2769,7 +2573,7 @@
         <v>/Companions/Fellow_DrakeChiefGuard.png</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2787,7 +2591,7 @@
         <v>/Companions/Fellow_Echo_Elder.png</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2805,7 +2609,7 @@
         <v>/Companions/Fellow_BlackSmith.png</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2823,7 +2627,7 @@
         <v>/Companions/Fellow_PengKintManager.png</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2841,7 +2645,7 @@
         <v>/Companions/Fellow_DevilStoneDismantler.png</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2859,7 +2663,7 @@
         <v>/Companions/Fellow_Zouk.png</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2877,7 +2681,7 @@
         <v>/Companions/Fellow_GodenZikus.png</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2895,7 +2699,7 @@
         <v>/Companions/Fellow_Kanoteon.png</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2913,7 +2717,7 @@
         <v>/Companions/Fellow_Tharsi.png</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2931,7 +2735,7 @@
         <v>/Companions/Fellow_Vivana.png</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2949,7 +2753,7 @@
         <v>/Companions/Fellow_Echo_OldWoman.png</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2967,7 +2771,7 @@
         <v>/Companions/Fellow_Tundra_Human_FatMan.png</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2985,7 +2789,7 @@
         <v>/Companions/Fellow_Tundra_Human_Woman.png</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3003,7 +2807,7 @@
         <v>/Companions/Fellow_Tundra_Human_Boy.png</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3021,7 +2825,7 @@
         <v>/Companions/Fellow_Tundra_Human.png</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3039,7 +2843,7 @@
         <v>/Companions/Fellow_Tundra_OldMan.png</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3057,7 +2861,7 @@
         <v>/Companions/Fellow_SkillBookMerchant2.png</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3086,213 +2890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94488B5-B1B1-4FD6-B124-C677D392D464}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.625" customWidth="1"/>
-    <col min="5" max="5" width="57.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="str">
-        <f t="shared" ref="E2:E8" si="0">"/GoldenApple/"&amp;B2&amp;".png"</f>
-        <v>/GoldenApple/GoldApple_auto-battle charge ticket (30 min).png</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/GoldApple_berzerker bon-bons.png</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/GoldApple_bottomless hp potion v2.0.png</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/GoldApple_fruity candy.png</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/GoldApple_Net's Pyramid Admission Ticket.png</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/GoldApple_Nett's pyramid Entry ticket.png</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>/GoldenApple/Mysterious weapon wheatstone (rare).png</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F3E161-477E-4EAE-9703-4AD284967BB0}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="39.75" customWidth="1"/>
     <col min="3" max="3" width="22.25" bestFit="1" customWidth="1"/>
@@ -3300,7 +2905,7 @@
     <col min="5" max="5" width="52.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -3316,16 +2921,16 @@
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>1</v>
@@ -3341,14 +2946,14 @@
         <f>"/UI/V4GB/"&amp;Table224[[#This Row],[StringID]]&amp;".jpg"</f>
         <v>/UI/V4GB/UI_V4Shop.jpg</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>2</v>
@@ -3364,14 +2969,14 @@
         <f>"/UI/V4GB/"&amp;Table224[[#This Row],[StringID]]&amp;".jpg"</f>
         <v>/UI/V4GB/UI_BurgerMenu.jpg</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>3</v>
@@ -3388,7 +2993,7 @@
         <v>/UI/V4GB/UI_Inventory.jpg</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>4</v>
@@ -3405,7 +3010,7 @@
         <v>/UI/V4GB/UI_CurrencyList.jpg</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>5</v>
@@ -3422,7 +3027,7 @@
         <v>/UI/V4GB/UI_Exit.jpg</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>6</v>
@@ -3439,7 +3044,7 @@
         <v>/UI/V4GB/UI_MountsShop.jpg</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>7</v>
@@ -3456,7 +3061,7 @@
         <v>/UI/V4GB/UI_CompanionsShop.jpg</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>8</v>
@@ -3473,7 +3078,7 @@
         <v>/UI/V4GB/UI_CompanionTestPackage.jpg</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>9</v>
@@ -3490,7 +3095,7 @@
         <v>/UI/V4GB/UI_Purchase990.jpg</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>10</v>
@@ -3507,7 +3112,7 @@
         <v>/UI/V4GB/UI_OpenAll.jpg</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>11</v>
@@ -3524,7 +3129,7 @@
         <v>/UI/V4GB/UI_TryAgain.jpg</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>12</v>
@@ -3541,7 +3146,7 @@
         <v>/UI/V4GB/UI_ViewResults.jpg</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>13</v>
@@ -3558,7 +3163,7 @@
         <v>/UI/V4GB/UI_Okay.jpg</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>14</v>
@@ -3575,16 +3180,16 @@
         <v>/UI/V4GB/UI_GachaFrame.jpg</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="str">
@@ -3592,16 +3197,16 @@
         <v>/UI/MSMG/UI_btn_Buy1.png</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4" t="str">
@@ -3609,16 +3214,16 @@
         <v>/UI/MSMG/UI_btn_Buy10.png</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4" t="str">
@@ -3626,16 +3231,16 @@
         <v>/UI/MSMG/UI_Btn_Cancel.png</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="4" t="str">
@@ -3643,16 +3248,16 @@
         <v>/UI/MSMG/UI_Btn_Confirm.png</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="4" t="str">
@@ -3660,16 +3265,16 @@
         <v>/UI/MSMG/UI_CheatMenu.png</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="4" t="str">
@@ -3677,16 +3282,16 @@
         <v>/UI/MSMG/UI_GoldenAppleSIDEMENU.png</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="4" t="str">
@@ -3694,16 +3299,16 @@
         <v>/UI/MSMG/UI_HambugerMENU.png</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="4" t="str">
@@ -3711,16 +3316,16 @@
         <v>/UI/MSMG/UI_Shop_CashShopMENU.png</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="4" t="str">
@@ -3728,16 +3333,16 @@
         <v>/UI/MSMG/UI_ShopMENU.png</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="str">
@@ -3745,16 +3350,16 @@
         <v>/UI/V4GB/UI_Console_OK.jpg</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="str">
@@ -3762,16 +3367,16 @@
         <v>/UI/V4GB/UI_NPCCheat.jpg</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="str">
@@ -3779,16 +3384,16 @@
         <v>/UI/V4GB/UI_Cheat_Input.jpg</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="str">
@@ -3796,16 +3401,16 @@
         <v>/UI/V4GB/UI_Create_NPC.jpg</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="str">
@@ -3813,16 +3418,16 @@
         <v>/UI/V4GB/UI_Cheat_Send.jpg</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <f>ROW(Table224[[#This Row],[Index]])-1</f>
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="str">
@@ -3830,19 +3435,19 @@
         <v>/UI/V4GB/UI_GeneralShop.jpg</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3858,7 +3463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="2"/>
@@ -3869,7 +3474,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="33.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
@@ -3877,1489 +3482,1489 @@
     <col min="6" max="6" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:3">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:3">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:3">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:3">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:3">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:3">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:3">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:3">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:3">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:3">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:3">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:3">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:3">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:3">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:3">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:3">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:3">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:3">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:3">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:3">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:3">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:3">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:3">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:3">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:3">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:3">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:3">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:3">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:3">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:3">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:3">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:3">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:3">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:3">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:3">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:3">
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:3">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:3">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:3">
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:3">
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:3">
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:3">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:3">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:3">
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:3">
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:3">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:3">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:3">
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:3">
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:3">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:3">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:3">
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:3">
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3">
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:3">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:3">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:3">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:3">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:3">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:3">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:3">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:3">
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:3">
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:3">
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:3">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:3">
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:3">
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:3">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:3">
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:3">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:3">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:3">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:3">
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:3">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:3">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:3">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:3">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:3">
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:3">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:3">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:3">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:3">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:3">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:3">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:3">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:3">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:3">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:3">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:3">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:3">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:3">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:3">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:3">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:3">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:3">
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:3">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:3">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:3">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:3">
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:3">
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:3">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:3">
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:3">
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:3">
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:3">
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:3">
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:3">
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:3">
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:3">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:3">
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:3">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:3">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:3">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:3">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:3">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:3">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:3">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:3">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:3">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:3">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:3">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:3">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:3">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:3">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:3">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:3">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:3">
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:3">
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:3">
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:3">
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:3">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:3">
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:3">
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:3">
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:3">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:3">
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:3">
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:3">
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:3">
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:3">
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:3">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:3">
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:3">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:3">
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:3">
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:3">
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:3">
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:3">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:3">
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:3">
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:3">
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:3">
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:3">
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:3">
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:3">
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:3">
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:3">
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:3">
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:3">
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:3">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:3">
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:3">
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:3">
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:3">
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:3">
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:3">
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:3">
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:3">
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:3">
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:3">
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:3">
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:3">
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:3">
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:3">
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:3">
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:3">
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:3">
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:3">
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:3">
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:3">
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:3">
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:3">
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:3">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:3">
       <c r="B276" s="1"/>
       <c r="C276" s="1"/>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:3">
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:3">
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:3">
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:3">
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:3">
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:3">
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:3">
       <c r="B283" s="1"/>
       <c r="C283" s="1"/>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:3">
       <c r="B284" s="1"/>
       <c r="C284" s="1"/>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:3">
       <c r="B285" s="1"/>
       <c r="C285" s="1"/>
     </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:3">
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
     </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:3">
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
     </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:3">
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:3">
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
     </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:3">
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
     </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:3">
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:3">
       <c r="B292" s="1"/>
       <c r="C292" s="1"/>
     </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:3">
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
     </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:3">
       <c r="B294" s="1"/>
       <c r="C294" s="1"/>
     </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:3">
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
     </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:3">
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
     </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:3">
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
     </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:3">
       <c r="B298" s="1"/>
       <c r="C298" s="1"/>
     </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:3">
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
     </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:3">
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
     </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:3">
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
     </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:3">
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
     </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:3">
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:3">
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:3">
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:3">
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:3">
       <c r="B307" s="1"/>
       <c r="C307" s="1"/>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:3">
       <c r="B308" s="1"/>
       <c r="C308" s="1"/>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:3">
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:3">
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:3">
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:3">
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:3">
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:3">
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:3">
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:3">
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:3">
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:3">
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:3">
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:3">
       <c r="B320" s="1"/>
       <c r="C320" s="1"/>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:3">
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:3">
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:3">
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:3">
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:3">
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:3">
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:3">
       <c r="B327" s="1"/>
       <c r="C327" s="1"/>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:3">
       <c r="B328" s="1"/>
       <c r="C328" s="1"/>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:3">
       <c r="B329" s="1"/>
       <c r="C329" s="1"/>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="330" spans="2:3">
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="331" spans="2:3">
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="332" spans="2:3">
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="333" spans="2:3">
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="334" spans="2:3">
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="335" spans="2:3">
       <c r="B335" s="1"/>
       <c r="C335" s="1"/>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="336" spans="2:3">
       <c r="B336" s="1"/>
       <c r="C336" s="1"/>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="337" spans="2:3">
       <c r="B337" s="1"/>
       <c r="C337" s="1"/>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="338" spans="2:3">
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
     </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="339" spans="2:3">
       <c r="B339" s="1"/>
       <c r="C339" s="1"/>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="340" spans="2:3">
       <c r="B340" s="1"/>
       <c r="C340" s="1"/>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="341" spans="2:3">
       <c r="B341" s="1"/>
       <c r="C341" s="1"/>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="342" spans="2:3">
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="343" spans="2:3">
       <c r="B343" s="1"/>
       <c r="C343" s="1"/>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="344" spans="2:3">
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="345" spans="2:3">
       <c r="B345" s="1"/>
       <c r="C345" s="1"/>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="346" spans="2:3">
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="347" spans="2:3">
       <c r="B347" s="1"/>
       <c r="C347" s="1"/>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="348" spans="2:3">
       <c r="B348" s="1"/>
       <c r="C348" s="1"/>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="349" spans="2:3">
       <c r="B349" s="1"/>
       <c r="C349" s="1"/>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="350" spans="2:3">
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="351" spans="2:3">
       <c r="B351" s="1"/>
       <c r="C351" s="1"/>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="352" spans="2:3">
       <c r="B352" s="1"/>
       <c r="C352" s="1"/>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="353" spans="2:3">
       <c r="B353" s="1"/>
       <c r="C353" s="1"/>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="354" spans="2:3">
       <c r="B354" s="1"/>
       <c r="C354" s="1"/>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="355" spans="2:3">
       <c r="B355" s="1"/>
       <c r="C355" s="1"/>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="356" spans="2:3">
       <c r="B356" s="1"/>
       <c r="C356" s="1"/>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="357" spans="2:3">
       <c r="B357" s="1"/>
       <c r="C357" s="1"/>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="358" spans="2:3">
       <c r="B358" s="1"/>
       <c r="C358" s="1"/>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="359" spans="2:3">
       <c r="B359" s="1"/>
       <c r="C359" s="1"/>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="360" spans="2:3">
       <c r="B360" s="1"/>
       <c r="C360" s="1"/>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="361" spans="2:3">
       <c r="B361" s="1"/>
       <c r="C361" s="1"/>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="362" spans="2:3">
       <c r="B362" s="1"/>
       <c r="C362" s="1"/>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="363" spans="2:3">
       <c r="B363" s="1"/>
       <c r="C363" s="1"/>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="364" spans="2:3">
       <c r="B364" s="1"/>
       <c r="C364" s="1"/>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="365" spans="2:3">
       <c r="B365" s="1"/>
       <c r="C365" s="1"/>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="366" spans="2:3">
       <c r="B366" s="1"/>
       <c r="C366" s="1"/>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="367" spans="2:3">
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="368" spans="2:3">
       <c r="B368" s="1"/>
       <c r="C368" s="1"/>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:3">
       <c r="B369" s="1"/>
       <c r="C369" s="1"/>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:3">
       <c r="B370" s="1"/>
       <c r="C370" s="1"/>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:3">
       <c r="B371" s="1"/>
       <c r="C371" s="1"/>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:3">
       <c r="B372" s="1"/>
       <c r="C372" s="1"/>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:3">
       <c r="B373" s="1"/>
       <c r="C373" s="1"/>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:3">
       <c r="B374" s="1"/>
       <c r="C374" s="1"/>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:3">
       <c r="B375" s="1"/>
       <c r="C375" s="1"/>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="376" spans="2:3">
       <c r="B376" s="1"/>
       <c r="C376" s="1"/>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="2:3">
       <c r="B377" s="1"/>
       <c r="C377" s="1"/>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:3">
       <c r="B378" s="1"/>
       <c r="C378" s="1"/>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:3">
       <c r="B379" s="1"/>
       <c r="C379" s="1"/>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:3">
       <c r="B380" s="1"/>
       <c r="C380" s="1"/>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:3">
       <c r="B381" s="1"/>
       <c r="C381" s="1"/>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:3">
       <c r="B382" s="1"/>
       <c r="C382" s="1"/>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:3">
       <c r="B383" s="1"/>
       <c r="C383" s="1"/>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:3">
       <c r="B384" s="1"/>
       <c r="C384" s="1"/>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="385" spans="2:3">
       <c r="B385" s="1"/>
       <c r="C385" s="1"/>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="386" spans="2:3">
       <c r="B386" s="1"/>
       <c r="C386" s="1"/>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="387" spans="2:3">
       <c r="B387" s="1"/>
       <c r="C387" s="1"/>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="388" spans="2:3">
       <c r="B388" s="1"/>
       <c r="C388" s="1"/>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="389" spans="2:3">
       <c r="B389" s="1"/>
       <c r="C389" s="1"/>
     </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="390" spans="2:3">
       <c r="B390" s="1"/>
       <c r="C390" s="1"/>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="391" spans="2:3">
       <c r="B391" s="1"/>
       <c r="C391" s="1"/>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="392" spans="2:3">
       <c r="B392" s="1"/>
       <c r="C392" s="1"/>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="393" spans="2:3">
       <c r="B393" s="1"/>
       <c r="C393" s="1"/>
     </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="394" spans="2:3">
       <c r="B394" s="1"/>
       <c r="C394" s="1"/>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="395" spans="2:3">
       <c r="B395" s="1"/>
       <c r="C395" s="1"/>
     </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="396" spans="2:3">
       <c r="B396" s="1"/>
       <c r="C396" s="1"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F1A9B88A-78B1-419F-A391-83B1454A44C5}">
+    <customSheetView guid="{92D4AFAD-54DB-4804-87A5-F807BA99876A}">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -5367,7 +4972,7 @@
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{92D4AFAD-54DB-4804-87A5-F807BA99876A}">
+    <customSheetView guid="{F1A9B88A-78B1-419F-A391-83B1454A44C5}">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -5377,7 +4982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3EEA2-4023-4C8C-AFFC-90438ED85D31}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5385,7 +4990,7 @@
       <selection activeCell="I22" sqref="I22:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
@@ -5395,7 +5000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB572F-0BCD-4AC1-AA89-CF0CE2E426D3}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5403,9 +5008,9 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>

</xml_diff>